<commit_message>
More edits to card text
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleylucouch/Documents/TRAAB_Cards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E6917A-71FE-6B47-A087-6230FD8FCD64}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D840D32-F522-7041-BC23-C67CFCA0AF21}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6460" yWindow="460" windowWidth="21940" windowHeight="17440" xr2:uid="{D5C866A4-9C33-EB4E-9D4B-68221F48654F}"/>
+    <workbookView xWindow="1220" yWindow="460" windowWidth="21940" windowHeight="17440" xr2:uid="{D5C866A4-9C33-EB4E-9D4B-68221F48654F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -549,9 +549,6 @@
     <t>Any player that card shares with you gains "shy" condition.</t>
   </si>
   <si>
-    <t>Must card share with the King before the end of the game or the Blue Team loses.</t>
-  </si>
-  <si>
     <t>You must card share with the President before the end of the last round.</t>
   </si>
   <si>
@@ -561,16 +558,10 @@
     <t>Take a player’s character card anytime they attempt to use a card share power on you. You are not affected by the card share power.</t>
   </si>
   <si>
-    <t>If you fail to card share with the King and Alchemist is "dead", the blue team looses.</t>
-  </si>
-  <si>
     <t>If your vote helped successfully usurp a leader during a majority of the rounds, you win.</t>
   </si>
   <si>
     <t>Announce “I am the Beholder!” You have the "Immune" condition, and can walk freely between the rooms.</t>
-  </si>
-  <si>
-    <t>If you announce when you see any part of a player’s card, you win. If you are wrong, you loose.</t>
   </si>
   <si>
     <t>You must always tell the truth.</t>
@@ -901,9 +892,6 @@
   </si>
   <si>
     <t>You are the backup character for the Engineer. If the Engineer gains the "dead" condition during the game or is buried, you take the role of the Engineer.</t>
-  </si>
-  <si>
-    <t>You are the backup character for the Alchemist. If the Alchemist gains the "dead" condition during the game or is buried, you must card share with the king.</t>
   </si>
   <si>
     <t>Who am I?</t>
@@ -1260,9 +1248,6 @@
     <t>You have the "tackle" power. Publicly reveal your card, pick any player in the room and say, "You're going nowhere." If the target is on the same team as you, they gain the "tackled" condition and can't leave as a hostage this round. Otherwise they gain the “torn” condition, and must publicly reveal their card.</t>
   </si>
   <si>
-    <t>At the end of the game, you must declare which team you are on. "I remember which team I am on. I am on the _ ." (Red Team, Blue Team, or neither) To win you want to guess the team allegiance of the buried card.</t>
-  </si>
-  <si>
     <t>If you choose the correct team, but your team loses, you lose. If you say, "I am on nobody's team," and you are correct, you win.</t>
   </si>
   <si>
@@ -1501,6 +1486,21 @@
   </si>
   <si>
     <t>I have unfinished business</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you see any part of another player’s card and can correctly announce it, you win. If you are wrong, you lose. </t>
+  </si>
+  <si>
+    <t>You are the backup character for the Alchemist. If The Alchemist gains the "dead" condition during the game or is buried, you must card share with the King.</t>
+  </si>
+  <si>
+    <t>If you fail to card share with the King and The Alchemist is "dead", the blue team loses.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At the end of the game, you must declare which team you are on by saying "I remember which team I am on. I am on the _." To win, you need to guess the allegiance of the buried card. </t>
+  </si>
+  <si>
+    <t>You must card share with the King before the end of the game.</t>
   </si>
 </sst>
 </file>
@@ -1889,10 +1889,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1319201-7300-864A-9EB3-B86618CE3873}">
   <dimension ref="A1:WHQ205"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A196" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="C205" sqref="C205"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1906,25 +1906,25 @@
   <sheetData>
     <row r="1" spans="1:15773" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>35</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:15773" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1935,13 +1935,13 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G2" s="1">
         <v>1</v>
@@ -1955,13 +1955,13 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
@@ -1972,13 +1972,13 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>34</v>
@@ -1992,13 +1992,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>1</v>
@@ -2018,13 +2018,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>172</v>
+        <v>489</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G6" s="1">
         <v>1</v>
@@ -64866,13 +64866,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>169</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
@@ -64886,13 +64886,13 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>169</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
@@ -64906,13 +64906,13 @@
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G9" s="1">
         <v>1</v>
@@ -64926,13 +64926,13 @@
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G10" s="1">
         <v>1</v>
@@ -64946,13 +64946,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>409</v>
+        <v>488</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>37</v>
@@ -64966,16 +64966,16 @@
         <v>58</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G12" s="1">
         <v>1</v>
@@ -64992,10 +64992,10 @@
         <v>40</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G13" s="1">
         <v>1</v>
@@ -65012,10 +65012,10 @@
         <v>40</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G14" s="1">
         <v>1</v>
@@ -65029,13 +65029,13 @@
         <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>290</v>
+        <v>486</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>176</v>
+        <v>487</v>
       </c>
       <c r="G15" s="1">
         <v>1</v>
@@ -65046,16 +65046,16 @@
         <v>60</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>179</v>
+        <v>485</v>
       </c>
       <c r="G16" s="1">
         <v>1</v>
@@ -65069,7 +65069,7 @@
         <v>61</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="G17" s="1">
         <v>1</v>
@@ -65083,13 +65083,13 @@
         <v>5</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G18" s="1">
         <v>1</v>
@@ -65103,13 +65103,13 @@
         <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G19" s="1">
         <v>1</v>
@@ -65123,10 +65123,10 @@
         <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>42</v>
@@ -65146,13 +65146,13 @@
         <v>5</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G21" s="1">
         <v>1</v>
@@ -65172,7 +65172,7 @@
         <v>44</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G22" s="1">
         <v>10</v>
@@ -65192,7 +65192,7 @@
         <v>168</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G23" s="1">
         <v>1</v>
@@ -65212,7 +65212,7 @@
         <v>168</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G24" s="1">
         <v>1</v>
@@ -65226,13 +65226,13 @@
         <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G25" s="1">
         <v>1</v>
@@ -65243,13 +65243,13 @@
         <v>16</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>47</v>
@@ -65266,13 +65266,13 @@
         <v>5</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>48</v>
@@ -65289,13 +65289,13 @@
         <v>6</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>48</v>
@@ -65312,13 +65312,13 @@
         <v>5</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G29" s="1">
         <v>1</v>
@@ -65332,13 +65332,13 @@
         <v>6</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G30" s="1">
         <v>1</v>
@@ -65349,16 +65349,16 @@
         <v>63</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G31" s="1">
         <v>1</v>
@@ -65372,13 +65372,13 @@
         <v>5</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G32" s="1">
         <v>1</v>
@@ -65392,13 +65392,13 @@
         <v>5</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>170</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G33" s="1">
         <v>1</v>
@@ -65412,13 +65412,13 @@
         <v>6</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>170</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G34" s="1">
         <v>1</v>
@@ -65429,16 +65429,16 @@
         <v>20</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G35" s="1">
         <v>1</v>
@@ -65446,19 +65446,19 @@
     </row>
     <row r="36" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G36" s="1">
         <v>1</v>
@@ -65466,19 +65466,19 @@
     </row>
     <row r="37" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G37" s="1">
         <v>1</v>
@@ -65486,36 +65486,36 @@
     </row>
     <row r="38" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="39" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G39" s="1">
         <v>1</v>
@@ -65523,19 +65523,19 @@
     </row>
     <row r="40" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G40" s="1">
         <v>1</v>
@@ -65549,13 +65549,13 @@
         <v>5</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>190</v>
-      </c>
       <c r="E41" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G41" s="1">
         <v>1</v>
@@ -65569,13 +65569,13 @@
         <v>6</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>190</v>
-      </c>
       <c r="E42" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G42" s="1">
         <v>1</v>
@@ -65589,13 +65589,13 @@
         <v>5</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G43" s="1">
         <v>1</v>
@@ -65609,13 +65609,13 @@
         <v>6</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G44" s="1">
         <v>1</v>
@@ -65629,13 +65629,13 @@
         <v>5</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>171</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G45" s="1">
         <v>1</v>
@@ -65649,13 +65649,13 @@
         <v>6</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>171</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G46" s="1">
         <v>1</v>
@@ -65666,16 +65666,16 @@
         <v>69</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="G47" s="1">
         <v>1</v>
@@ -65689,10 +65689,10 @@
         <v>6</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="G48" s="1">
         <v>1</v>
@@ -65706,13 +65706,13 @@
         <v>5</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G49" s="1">
         <v>1</v>
@@ -65726,13 +65726,13 @@
         <v>6</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G50" s="1">
         <v>1</v>
@@ -65743,13 +65743,13 @@
         <v>22</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>50</v>
@@ -65769,13 +65769,13 @@
         <v>5</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G52" s="1">
         <v>1</v>
@@ -65789,13 +65789,13 @@
         <v>6</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G53" s="1">
         <v>1</v>
@@ -65809,10 +65809,10 @@
         <v>5</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>51</v>
@@ -65829,13 +65829,13 @@
         <v>6</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G55" s="1">
         <v>1</v>
@@ -65849,13 +65849,13 @@
         <v>6</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G56" s="1">
         <v>1</v>
@@ -65869,13 +65869,13 @@
         <v>6</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G57" s="1">
         <v>1</v>
@@ -65889,13 +65889,13 @@
         <v>8</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="G58" s="1">
         <v>1</v>
@@ -65906,16 +65906,16 @@
         <v>71</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>217</v>
-      </c>
       <c r="D59" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G59" s="1">
         <v>1</v>
@@ -65929,13 +65929,13 @@
         <v>6</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="G60" s="1">
         <v>1</v>
@@ -65949,13 +65949,13 @@
         <v>5</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G61" s="1">
         <v>1</v>
@@ -65969,13 +65969,13 @@
         <v>6</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G62" s="1">
         <v>1</v>
@@ -65989,13 +65989,13 @@
         <v>5</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G63" s="1">
         <v>1</v>
@@ -66009,13 +66009,13 @@
         <v>5</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G64" s="1">
         <v>1</v>
@@ -66029,13 +66029,13 @@
         <v>6</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G65" s="1">
         <v>1</v>
@@ -66049,13 +66049,13 @@
         <v>5</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G66" s="1">
         <v>1</v>
@@ -66069,13 +66069,13 @@
         <v>5</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G67" s="1">
         <v>1</v>
@@ -66089,13 +66089,13 @@
         <v>6</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G68" s="1">
         <v>1</v>
@@ -66109,13 +66109,13 @@
         <v>6</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="G69" s="1">
         <v>1</v>
@@ -66126,16 +66126,16 @@
         <v>82</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="G70" s="1">
         <v>1</v>
@@ -66149,13 +66149,13 @@
         <v>5</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G71" s="1">
         <v>1</v>
@@ -66169,13 +66169,13 @@
         <v>5</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G72" s="1">
         <v>1</v>
@@ -66189,13 +66189,13 @@
         <v>5</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G73" s="1">
         <v>1</v>
@@ -66209,13 +66209,13 @@
         <v>6</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G74" s="1">
         <v>1</v>
@@ -66226,7 +66226,7 @@
         <v>27</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>32</v>
@@ -66249,13 +66249,13 @@
         <v>6</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="G76" s="1">
         <v>1</v>
@@ -66266,16 +66266,16 @@
         <v>29</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>56</v>
@@ -66289,16 +66289,16 @@
         <v>86</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G78" s="1">
         <v>3</v>
@@ -66312,13 +66312,13 @@
         <v>5</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G79" s="1">
         <v>1</v>
@@ -66332,13 +66332,13 @@
         <v>6</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G80" s="1">
         <v>1</v>
@@ -66352,13 +66352,13 @@
         <v>5</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G81" s="1">
         <v>1</v>
@@ -66372,13 +66372,13 @@
         <v>6</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G82" s="1">
         <v>1</v>
@@ -66386,19 +66386,19 @@
     </row>
     <row r="83" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="84" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -66409,13 +66409,13 @@
         <v>5</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G84" s="1">
         <v>1</v>
@@ -66429,13 +66429,13 @@
         <v>6</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G85" s="1">
         <v>1</v>
@@ -66446,16 +66446,16 @@
         <v>89</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="G86" s="1">
         <v>1</v>
@@ -66466,16 +66466,16 @@
         <v>90</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="G87" s="1">
         <v>1</v>
@@ -66489,13 +66489,13 @@
         <v>5</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G88" s="1">
         <v>1</v>
@@ -66509,13 +66509,13 @@
         <v>6</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G89" s="1">
         <v>1</v>
@@ -66529,13 +66529,13 @@
         <v>5</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G90" s="1">
         <v>1</v>
@@ -66549,13 +66549,13 @@
         <v>6</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G91" s="1">
         <v>1</v>
@@ -66569,13 +66569,13 @@
         <v>5</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G92" s="1">
         <v>1</v>
@@ -66589,13 +66589,13 @@
         <v>6</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G93" s="1">
         <v>1</v>
@@ -66609,13 +66609,13 @@
         <v>5</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G94" s="1">
         <v>1</v>
@@ -66629,13 +66629,13 @@
         <v>6</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G95" s="1">
         <v>1</v>
@@ -66646,16 +66646,16 @@
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G96" s="1">
         <v>1</v>
@@ -66669,13 +66669,13 @@
         <v>5</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G97" s="1">
         <v>1</v>
@@ -66689,13 +66689,13 @@
         <v>6</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G98" s="1">
         <v>1</v>
@@ -66706,16 +66706,16 @@
         <v>97</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="G99" s="1">
         <v>1</v>
@@ -66726,16 +66726,16 @@
         <v>98</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G100" s="1">
         <v>1</v>
@@ -66749,13 +66749,13 @@
         <v>5</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G101" s="1">
         <v>1</v>
@@ -66769,13 +66769,13 @@
         <v>6</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G102" s="1">
         <v>1</v>
@@ -66789,13 +66789,13 @@
         <v>5</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="G103" s="1">
         <v>1</v>
@@ -66806,16 +66806,16 @@
         <v>101</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G104" s="1">
         <v>1</v>
@@ -66829,13 +66829,13 @@
         <v>5</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G105" s="1">
         <v>1</v>
@@ -66849,13 +66849,13 @@
         <v>6</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G106" s="1">
         <v>1</v>
@@ -66869,13 +66869,13 @@
         <v>5</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G107" s="1">
         <v>1</v>
@@ -66889,13 +66889,13 @@
         <v>6</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G108" s="1">
         <v>1</v>
@@ -66906,16 +66906,16 @@
         <v>104</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G109" s="1">
         <v>1</v>
@@ -66929,13 +66929,13 @@
         <v>5</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="G110" s="1">
         <v>1</v>
@@ -66949,13 +66949,13 @@
         <v>6</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G111" s="1">
         <v>1</v>
@@ -66969,13 +66969,13 @@
         <v>5</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G112" s="1">
         <v>1</v>
@@ -66989,13 +66989,13 @@
         <v>6</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G113" s="1">
         <v>1</v>
@@ -67009,13 +67009,13 @@
         <v>5</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G114" s="1">
         <v>1</v>
@@ -67029,13 +67029,13 @@
         <v>6</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G115" s="1">
         <v>1</v>
@@ -67046,16 +67046,16 @@
         <v>110</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="G116" s="1">
         <v>1</v>
@@ -67069,13 +67069,13 @@
         <v>5</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G117" s="1">
         <v>1</v>
@@ -67089,13 +67089,13 @@
         <v>6</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G118" s="1">
         <v>1</v>
@@ -67106,13 +67106,13 @@
         <v>112</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>31</v>
@@ -67126,16 +67126,16 @@
         <v>113</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="G120" s="1">
         <v>1</v>
@@ -67146,16 +67146,16 @@
         <v>36</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="G121" s="1">
         <v>1</v>
@@ -67166,16 +67166,16 @@
         <v>114</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="G122" s="1">
         <v>1</v>
@@ -67189,13 +67189,13 @@
         <v>5</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G123" s="1">
         <v>1</v>
@@ -67209,13 +67209,13 @@
         <v>6</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G124" s="1">
         <v>1</v>
@@ -67229,13 +67229,13 @@
         <v>5</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G125" s="1">
         <v>1</v>
@@ -67249,13 +67249,13 @@
         <v>6</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G126" s="1">
         <v>1</v>
@@ -67269,13 +67269,13 @@
         <v>5</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G127" s="1">
         <v>1</v>
@@ -67289,13 +67289,13 @@
         <v>6</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G128" s="1">
         <v>1</v>
@@ -67306,16 +67306,16 @@
         <v>118</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G129" s="1">
         <v>1</v>
@@ -67329,13 +67329,13 @@
         <v>5</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G130" s="1">
         <v>1</v>
@@ -67349,13 +67349,13 @@
         <v>5</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G131" s="1">
         <v>1</v>
@@ -67369,13 +67369,13 @@
         <v>5</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G132" s="1">
         <v>1</v>
@@ -67389,13 +67389,13 @@
         <v>6</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G133" s="1">
         <v>1</v>
@@ -67406,16 +67406,16 @@
         <v>122</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G134" s="1">
         <v>1</v>
@@ -67429,13 +67429,13 @@
         <v>5</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G135" s="1">
         <v>1</v>
@@ -67449,13 +67449,13 @@
         <v>6</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G136" s="1">
         <v>1</v>
@@ -67469,13 +67469,13 @@
         <v>5</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G137" s="1">
         <v>1</v>
@@ -67489,13 +67489,13 @@
         <v>6</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G138" s="1">
         <v>1</v>
@@ -67509,13 +67509,13 @@
         <v>5</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G139" s="1">
         <v>1</v>
@@ -67529,13 +67529,13 @@
         <v>6</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G140" s="1">
         <v>1</v>
@@ -67549,13 +67549,13 @@
         <v>5</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G141" s="1">
         <v>1</v>
@@ -67569,13 +67569,13 @@
         <v>5</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G142" s="1">
         <v>1</v>
@@ -67586,16 +67586,16 @@
         <v>128</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="G143" s="1">
         <v>1</v>
@@ -67609,13 +67609,13 @@
         <v>5</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G144" s="1">
         <v>1</v>
@@ -67629,13 +67629,13 @@
         <v>6</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G145" s="1">
         <v>1</v>
@@ -67646,16 +67646,16 @@
         <v>56</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="G146" s="1">
         <v>1</v>
@@ -67669,13 +67669,13 @@
         <v>5</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G147" s="1">
         <v>1</v>
@@ -67689,13 +67689,13 @@
         <v>6</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G148" s="1">
         <v>1</v>
@@ -67709,13 +67709,13 @@
         <v>6</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G149" s="1">
         <v>1</v>
@@ -67726,16 +67726,16 @@
         <v>132</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G150" s="1">
         <v>1</v>
@@ -67749,13 +67749,13 @@
         <v>5</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G151" s="1">
         <v>1</v>
@@ -67769,13 +67769,13 @@
         <v>6</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G152" s="1">
         <v>1</v>
@@ -67789,10 +67789,10 @@
         <v>5</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G153" s="1">
         <v>1</v>
@@ -67806,10 +67806,10 @@
         <v>6</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G154" s="1">
         <v>1</v>
@@ -67823,13 +67823,13 @@
         <v>6</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G155" s="1">
         <v>1</v>
@@ -67843,13 +67843,13 @@
         <v>6</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G156" s="1">
         <v>1</v>
@@ -67866,10 +67866,10 @@
         <v>9</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G157" s="1">
         <v>10</v>
@@ -67880,16 +67880,16 @@
         <v>137</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G158" s="1">
         <v>1</v>
@@ -67900,16 +67900,16 @@
         <v>138</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G159" s="1">
         <v>1</v>
@@ -67920,16 +67920,16 @@
         <v>139</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G160" s="1">
         <v>1</v>
@@ -67940,16 +67940,16 @@
         <v>140</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="G161" s="1">
         <v>1</v>
@@ -67960,16 +67960,16 @@
         <v>141</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G162" s="1">
         <v>1</v>
@@ -67980,16 +67980,16 @@
         <v>142</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="G163" s="1">
         <v>1</v>
@@ -68003,13 +68003,13 @@
         <v>5</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="G164" s="1">
         <v>1</v>
@@ -68023,13 +68023,13 @@
         <v>6</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="G165" s="1">
         <v>1</v>
@@ -68043,13 +68043,13 @@
         <v>5</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G166" s="1">
         <v>1</v>
@@ -68063,13 +68063,13 @@
         <v>6</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G167" s="1">
         <v>1</v>
@@ -68083,13 +68083,13 @@
         <v>5</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G168" s="1">
         <v>1</v>
@@ -68103,13 +68103,13 @@
         <v>6</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G169" s="1">
         <v>1</v>
@@ -68123,13 +68123,13 @@
         <v>5</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G170" s="1">
         <v>1</v>
@@ -68143,13 +68143,13 @@
         <v>6</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G171" s="1">
         <v>1</v>
@@ -68163,13 +68163,13 @@
         <v>6</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G172" s="1">
         <v>1</v>
@@ -68183,13 +68183,13 @@
         <v>5</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G173" s="1">
         <v>1</v>
@@ -68203,13 +68203,13 @@
         <v>6</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G174" s="1">
         <v>1</v>
@@ -68220,16 +68220,16 @@
         <v>149</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G175" s="1">
         <v>1</v>
@@ -68240,16 +68240,16 @@
         <v>150</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="G176" s="1">
         <v>1</v>
@@ -68260,16 +68260,16 @@
         <v>151</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="G177" s="1">
         <v>1</v>
@@ -68280,16 +68280,16 @@
         <v>152</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="G178" s="1">
         <v>1</v>
@@ -68303,13 +68303,13 @@
         <v>5</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G179" s="1">
         <v>1</v>
@@ -68323,13 +68323,13 @@
         <v>6</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G180" s="1">
         <v>1</v>
@@ -68343,13 +68343,13 @@
         <v>5</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G181" s="1">
         <v>1</v>
@@ -68363,13 +68363,13 @@
         <v>6</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G182" s="1">
         <v>1</v>
@@ -68383,10 +68383,10 @@
         <v>6</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="G183" s="1">
         <v>1</v>
@@ -68400,13 +68400,13 @@
         <v>5</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G184" s="1">
         <v>1</v>
@@ -68420,13 +68420,13 @@
         <v>6</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G185" s="1">
         <v>1</v>
@@ -68437,16 +68437,16 @@
         <v>157</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="G186" s="1">
         <v>1</v>
@@ -68460,13 +68460,13 @@
         <v>5</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="G187" s="1">
         <v>1</v>
@@ -68480,13 +68480,13 @@
         <v>5</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G188" s="1">
         <v>1</v>
@@ -68500,13 +68500,13 @@
         <v>6</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G189" s="1">
         <v>1</v>
@@ -68520,13 +68520,13 @@
         <v>5</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G190" s="1">
         <v>1</v>
@@ -68540,13 +68540,13 @@
         <v>6</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G191" s="1">
         <v>1</v>
@@ -68557,16 +68557,16 @@
         <v>161</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="G192" s="1">
         <v>1</v>
@@ -68577,16 +68577,16 @@
         <v>162</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="G193" s="1">
         <v>1</v>
@@ -68600,13 +68600,13 @@
         <v>5</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G194" s="1">
         <v>1</v>
@@ -68620,13 +68620,13 @@
         <v>6</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G195" s="1">
         <v>1</v>
@@ -68640,13 +68640,13 @@
         <v>5</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G196" s="1">
         <v>1</v>
@@ -68660,13 +68660,13 @@
         <v>6</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G197" s="1">
         <v>1</v>
@@ -68677,16 +68677,16 @@
         <v>165</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="G198" s="1">
         <v>1</v>
@@ -68700,13 +68700,13 @@
         <v>6</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="G199" s="1">
         <v>1</v>
@@ -68717,16 +68717,16 @@
         <v>167</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="G200" s="1">
         <v>1</v>
@@ -68734,19 +68734,19 @@
     </row>
     <row r="201" spans="1:8" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="G201" s="1">
         <v>1</v>
@@ -68766,7 +68766,7 @@
         <v>106</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="G203" s="1">
         <v>0</v>
@@ -68793,5 +68793,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Edits to card text, and adding Mastermind and Illuminati
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewmccaskill/Documents/TRAAB_Cards/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleylucouch/Documents/TRAAB_Cards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849EA6D6-B472-2B45-AA57-AFF9CA7D049B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376D8C88-77BA-1D4C-BFA8-DFFCB79D090D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="-3140" windowWidth="38400" windowHeight="21140" xr2:uid="{D5C866A4-9C33-EB4E-9D4B-68221F48654F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19200" xr2:uid="{D5C866A4-9C33-EB4E-9D4B-68221F48654F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="509">
   <si>
     <t>AGORAPHOBE</t>
   </si>
@@ -597,9 +597,6 @@
     <t>If you are in the same room as Juliet and the Bomber at the end of the game, you win.</t>
   </si>
   <si>
-    <t>Any player that card shares with you must trade in their character card for a Blue Team card before the beginning of the next round and before revealing any part of their card to another player.</t>
-  </si>
-  <si>
     <t>You are a member of the Red Team, your goal is aligned with that of the Red Team.</t>
   </si>
   <si>
@@ -721,9 +718,6 @@
   </si>
   <si>
     <t>Next in line</t>
-  </si>
-  <si>
-    <t>Keep your head down</t>
   </si>
   <si>
     <t>Let's talk</t>
@@ -1008,9 +1002,6 @@
     <t>There can only be one</t>
   </si>
   <si>
-    <t>Give me my sin again</t>
-  </si>
-  <si>
     <t>Always watching</t>
   </si>
   <si>
@@ -1018,9 +1009,6 @@
   </si>
   <si>
     <t>I know your thoughts</t>
-  </si>
-  <si>
-    <t>I know what you're thinking</t>
   </si>
   <si>
     <t>I know what you dream of</t>
@@ -1153,9 +1141,6 @@
   </si>
   <si>
     <t>Once per round, you may privately reveal your card simultaneously to two players. These players must card share to each other (but not to you).</t>
-  </si>
-  <si>
-    <t>You begin with the "flashing" condition: you may only publicly reveal, even with another character's power might force a color share, card share, or private reveal.</t>
   </si>
   <si>
     <t>If you card share with the President, they gain the "fireproof" condition. If the President has the fireproof condition at the end of the game, all players in the same room as the President gain the "fireproof" condition: they do not gain the "dead" condition from the "firebomb" condition.</t>
@@ -1365,9 +1350,6 @@
     <t>You may publicly reveal your card at any time and verbally announce, "Time is up!" to immediately end the round. Be sure that both rooms hear the call to end the round. If you take longer than 5 minutes to call a round, you lose this power.</t>
   </si>
   <si>
-    <t>You have the "trade" power: you may trade your card for the buried card. You may not peek at the buried card, only trade with it, and you assume all powers and the allegiance of your newly acquired card. The "trade" power can be used by any player only once per round.</t>
-  </si>
-  <si>
     <t>If you are sent to a different room as a hostage at the end of a majority of the rounds, you win.</t>
   </si>
   <si>
@@ -1375,9 +1357,6 @@
   </si>
   <si>
     <t>If you card share with the Bomber (does not include the Martyr), the game immediately ends, Blue Team wins, and Red Team loses.</t>
-  </si>
-  <si>
-    <t>Any player who card shares with you that has a color not of your own gains the "seduced" condition. All "seduced" players must do anything with their card that you ask of them and must vote for or against leaders as you do.</t>
   </si>
   <si>
     <t>You are one of the two alpha wolves and have the "werewolf" power. Any player that card shares or color shares with you or someone with the "bitten" condition gains the "bitten" condition: they must answer any question either of the alpha wolves ask as honestly and informatively as possible.</t>
@@ -1416,12 +1395,6 @@
     <t>Right.</t>
   </si>
   <si>
-    <t>If you win, all other players lose.</t>
-  </si>
-  <si>
-    <t>If any player color shares or card shares with you, you win.</t>
-  </si>
-  <si>
     <t>Before the game begins, but after character cards have been dealt, all players but Seers must close their eyes and publicly reveal their cards for 30 seconds. You begin with the "shy" condition: you may not reveal any part of your card to any player.</t>
   </si>
   <si>
@@ -1453,9 +1426,6 @@
   </si>
   <si>
     <t>If, at the end of the game, you are in the same room as Paper, but the opposite rooms as Rock, you win.</t>
-  </si>
-  <si>
-    <t>If, at the end of the game, you are in the same room as the President, but opposite room as the Bomber, you win.</t>
   </si>
   <si>
     <t>Any player that card shares with you trades cards with you and then acquires the "shy" condition: they may not reveal any part of their card to any player. They assume the allegiance of the Identity Thief card, and you assume the powers, allegiance, win objectives, and all starting conditions of the newly stolen card.</t>
@@ -1533,20 +1503,68 @@
     <t>If you, acting as the Alchemist, fail to card share with the acting King before the end of the game, Blue Team loses.</t>
   </si>
   <si>
-    <t>If you, acting as the Eggineer, fail to card share with the acting Dragon before the end of the game, Blue Team loses.</t>
-  </si>
-  <si>
     <t>You are the backup character for the King. If the King gains the "toast" condition during the game or is buried, you take the role of the King.</t>
   </si>
   <si>
     <t>I am the gate</t>
+  </si>
+  <si>
+    <t>You begin with the "flashing" condition: you may only publicly reveal, even when another character's power might force a color share, card share, or private reveal.</t>
+  </si>
+  <si>
+    <t>If you, acting as the Eggineer, fail to card share with the acting Dragon before the end of the game, Red Team loses.</t>
+  </si>
+  <si>
+    <t>Keep your head down, Sir</t>
+  </si>
+  <si>
+    <t>Thus with a kiss I die</t>
+  </si>
+  <si>
+    <t>Any player that card shares with you must trade in their character card for a Red Team card before the beginning of the next round and before revealing any part of their card to another player. (Your power has no effect on primary characters, backup characters, or non- Red/Blue Characters.)</t>
+  </si>
+  <si>
+    <t>Any player that card shares with you must trade in their character card for a Blue Team card before the beginning of the next round and before revealing any part of their card to another player. (Your power has no effect on primary characters, backup characters, or non- Red/Blue Characters.)</t>
+  </si>
+  <si>
+    <t>I know what you're planning</t>
+  </si>
+  <si>
+    <t>You have the "trade" power: you may trade your card for the buried card. You may not peek at the buried card, only trade with it, and you assume all powers and the allegiance of your newly acquired card. The "trade" power can be used by the Trader once per round.</t>
+  </si>
+  <si>
+    <t>You have the "seductive" power: any player who card shares with you that has a color not of your own gains the "seduced" condition: "seduced" players must do anything with their card that you ask of them and must vote for or against leaders as you do.</t>
+  </si>
+  <si>
+    <t>If, at the end of the game, you are in the same room as the President, but opposite room as the Bomber, you win. If you win, both the Red and Blue Team lose.</t>
+  </si>
+  <si>
+    <t>If any player color shares or card shares with you, you win. If you win, all other players lose.</t>
+  </si>
+  <si>
+    <t>Mastermind</t>
+  </si>
+  <si>
+    <t>If any player card shares with you then you win and all other players lose.</t>
+  </si>
+  <si>
+    <t>Illuminati</t>
+  </si>
+  <si>
+    <t>At the end of the last round, before all players reveal their cards, you must publicly announce the color of EVERY player. If you are able to correctly name the color of every player’s character card, then you win and all other players lose. If you get guess just 1 player’s color wrong, then you lose the game.</t>
+  </si>
+  <si>
+    <t>If you end the game as a room’s leader AND was a leader of the opposing room, you win.</t>
+  </si>
+  <si>
+    <t>You've fallen into my trap</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1576,21 +1594,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="14"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1609,6 +1619,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1622,7 +1650,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1632,10 +1660,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1950,12 +1980,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1319201-7300-864A-9EB3-B86618CE3873}">
-  <dimension ref="A1:WHQ206"/>
+  <dimension ref="A1:WHQ209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A187" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="C206" sqref="C206"/>
+      <selection pane="bottomLeft" activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1998,13 +2028,13 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G2" s="1">
         <v>1</v>
@@ -2018,13 +2048,13 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
@@ -2038,13 +2068,13 @@
         <v>168</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="G4" s="1">
         <v>1</v>
@@ -2058,10 +2088,10 @@
         <v>168</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>1</v>
@@ -2081,13 +2111,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>496</v>
+        <v>486</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>497</v>
+        <v>487</v>
       </c>
       <c r="G6" s="1">
         <v>1</v>
@@ -64929,13 +64959,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
@@ -64949,13 +64979,13 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
@@ -64969,13 +64999,13 @@
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G9" s="1">
         <v>1</v>
@@ -64989,13 +65019,13 @@
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G10" s="1">
         <v>1</v>
@@ -65009,13 +65039,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>32</v>
@@ -65032,13 +65062,13 @@
         <v>168</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>343</v>
       </c>
       <c r="G12" s="1">
         <v>1</v>
@@ -65055,10 +65085,10 @@
         <v>34</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G13" s="1">
         <v>1</v>
@@ -65075,10 +65105,10 @@
         <v>34</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G14" s="1">
         <v>1</v>
@@ -65092,13 +65122,13 @@
         <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>498</v>
+        <v>488</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>499</v>
+        <v>489</v>
       </c>
       <c r="G15" s="1">
         <v>1</v>
@@ -65112,13 +65142,13 @@
         <v>155</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="G16" s="1">
         <v>1</v>
@@ -65132,13 +65162,13 @@
         <v>5</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G17" s="1">
         <v>1</v>
@@ -65152,13 +65182,13 @@
         <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G18" s="1">
         <v>1</v>
@@ -65172,13 +65202,13 @@
         <v>5</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>39</v>
@@ -65188,20 +65218,20 @@
       </c>
     </row>
     <row r="20" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>483</v>
+        <v>473</v>
       </c>
       <c r="G20" s="1">
         <v>1</v>
@@ -65209,19 +65239,19 @@
     </row>
     <row r="21" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G21" s="1">
         <v>10</v>
@@ -65238,10 +65268,10 @@
         <v>35</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G22" s="1">
         <v>1</v>
@@ -65258,10 +65288,10 @@
         <v>35</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G23" s="1">
         <v>1</v>
@@ -65275,16 +65305,16 @@
         <v>6</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>481</v>
+        <v>471</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G24" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -65298,7 +65328,7 @@
         <v>152</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>36</v>
@@ -65315,13 +65345,13 @@
         <v>5</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>37</v>
@@ -65338,13 +65368,13 @@
         <v>6</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>37</v>
@@ -65361,13 +65391,13 @@
         <v>5</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>153</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G28" s="1">
         <v>1</v>
@@ -65381,13 +65411,13 @@
         <v>6</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>153</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G29" s="1">
         <v>1</v>
@@ -65401,10 +65431,10 @@
         <v>168</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>154</v>
@@ -65421,13 +65451,13 @@
         <v>5</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>188</v>
+        <v>235</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>497</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G31" s="1">
         <v>1</v>
@@ -65444,10 +65474,10 @@
         <v>156</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G32" s="1">
         <v>1</v>
@@ -65464,10 +65494,10 @@
         <v>156</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G33" s="1">
         <v>1</v>
@@ -65481,10 +65511,10 @@
         <v>168</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>173</v>
@@ -65495,19 +65525,19 @@
     </row>
     <row r="35" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G35" s="1">
         <v>1</v>
@@ -65515,19 +65545,19 @@
     </row>
     <row r="36" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G36" s="1">
         <v>1</v>
@@ -65535,19 +65565,19 @@
     </row>
     <row r="37" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>168</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="G37" s="1">
         <v>1</v>
@@ -65555,7 +65585,7 @@
     </row>
     <row r="38" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>5</v>
@@ -65564,10 +65594,10 @@
         <v>158</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G38" s="1">
         <v>1</v>
@@ -65575,7 +65605,7 @@
     </row>
     <row r="39" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>6</v>
@@ -65584,10 +65614,10 @@
         <v>158</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G39" s="1">
         <v>1</v>
@@ -65600,14 +65630,14 @@
       <c r="B40" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="10" t="s">
         <v>157</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G40" s="1">
         <v>1</v>
@@ -65620,14 +65650,14 @@
       <c r="B41" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="10" t="s">
         <v>157</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G41" s="1">
         <v>1</v>
@@ -65641,13 +65671,13 @@
         <v>5</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G42" s="1">
         <v>1</v>
@@ -65661,13 +65691,13 @@
         <v>6</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G43" s="1">
         <v>1</v>
@@ -65681,13 +65711,13 @@
         <v>5</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G44" s="1">
         <v>1</v>
@@ -65701,13 +65731,13 @@
         <v>6</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G45" s="1">
         <v>1</v>
@@ -65724,10 +65754,10 @@
         <v>159</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="G46" s="1">
         <v>1</v>
@@ -65741,13 +65771,13 @@
         <v>6</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G47" s="1">
         <v>1</v>
@@ -65761,13 +65791,13 @@
         <v>5</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G48" s="1">
         <v>1</v>
@@ -65781,13 +65811,13 @@
         <v>6</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G49" s="1">
         <v>1</v>
@@ -65801,13 +65831,13 @@
         <v>168</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>38</v>
@@ -65824,13 +65854,13 @@
         <v>5</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G51" s="1">
         <v>1</v>
@@ -65844,13 +65874,13 @@
         <v>6</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G52" s="1">
         <v>1</v>
@@ -65864,13 +65894,13 @@
         <v>5</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>495</v>
+        <v>485</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>480</v>
+        <v>470</v>
       </c>
       <c r="G53" s="1">
         <v>1</v>
@@ -65884,13 +65914,13 @@
         <v>6</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G54" s="1">
         <v>1</v>
@@ -65904,13 +65934,13 @@
         <v>6</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>488</v>
+        <v>478</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>489</v>
+        <v>479</v>
       </c>
       <c r="G55" s="1">
         <v>1</v>
@@ -65924,13 +65954,13 @@
         <v>6</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>489</v>
+        <v>479</v>
       </c>
       <c r="G56" s="1">
         <v>1</v>
@@ -65944,13 +65974,13 @@
         <v>8</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G57" s="1">
         <v>1</v>
@@ -65967,10 +65997,10 @@
         <v>170</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="G58" s="1">
         <v>1</v>
@@ -65984,13 +66014,13 @@
         <v>6</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>492</v>
+        <v>482</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>493</v>
+        <v>483</v>
       </c>
       <c r="G59" s="1">
         <v>1</v>
@@ -66004,13 +66034,13 @@
         <v>5</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G60" s="1">
         <v>1</v>
@@ -66024,13 +66054,13 @@
         <v>6</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G61" s="1">
         <v>1</v>
@@ -66040,17 +66070,17 @@
       <c r="A62" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>5</v>
+      <c r="B62" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>494</v>
+        <v>484</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>490</v>
+        <v>480</v>
       </c>
       <c r="G62" s="1">
         <v>1</v>
@@ -66067,7 +66097,10 @@
         <v>171</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>468</v>
+        <v>459</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>340</v>
       </c>
       <c r="G63" s="1">
         <v>1</v>
@@ -66084,10 +66117,10 @@
         <v>171</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G64" s="1">
         <v>1</v>
@@ -66101,13 +66134,13 @@
         <v>5</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G65" s="1">
         <v>1</v>
@@ -66121,13 +66154,13 @@
         <v>5</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>374</v>
+        <v>253</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>492</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G66" s="1">
         <v>1</v>
@@ -66141,13 +66174,13 @@
         <v>6</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>374</v>
+        <v>253</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>492</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G67" s="1">
         <v>1</v>
@@ -66161,13 +66194,13 @@
         <v>6</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E68" s="1" t="s">
-        <v>500</v>
+      <c r="E68" s="5" t="s">
+        <v>493</v>
       </c>
       <c r="G68" s="1">
         <v>1</v>
@@ -66181,13 +66214,13 @@
         <v>5</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>487</v>
+        <v>477</v>
       </c>
       <c r="G69" s="1">
         <v>1</v>
@@ -66201,13 +66234,13 @@
         <v>168</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="G70" s="1">
         <v>1</v>
@@ -66221,37 +66254,36 @@
         <v>5</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G71" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A72" s="9" t="s">
+      <c r="A72" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B72" s="9" t="s">
+      <c r="B72" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C72" s="9" t="s">
+      <c r="C72" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D72" s="9" t="s">
-        <v>339</v>
-      </c>
-      <c r="E72" s="9" t="s">
-        <v>376</v>
-      </c>
-      <c r="F72" s="9"/>
-      <c r="G72" s="9">
-        <v>0</v>
+      <c r="D72" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="G72" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -66262,13 +66294,13 @@
         <v>5</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G73" s="1">
         <v>1</v>
@@ -66282,13 +66314,13 @@
         <v>6</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G74" s="1">
         <v>1</v>
@@ -66305,10 +66337,10 @@
         <v>40</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>41</v>
@@ -66325,13 +66357,13 @@
         <v>6</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G76" s="1">
         <v>1</v>
@@ -66345,10 +66377,10 @@
         <v>168</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>172</v>
@@ -66365,13 +66397,13 @@
         <v>5</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G78" s="1">
         <v>1</v>
@@ -66385,13 +66417,13 @@
         <v>6</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G79" s="1">
         <v>1</v>
@@ -66405,13 +66437,13 @@
         <v>5</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G80" s="1">
         <v>1</v>
@@ -66425,13 +66457,13 @@
         <v>6</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G81" s="1">
         <v>1</v>
@@ -66439,16 +66471,16 @@
     </row>
     <row r="82" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>168</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>173</v>
@@ -66465,30 +66497,30 @@
         <v>168</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="G83" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A84" s="8" t="s">
+      <c r="A84" s="7" t="s">
         <v>75</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>168</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>173</v>
@@ -66508,10 +66540,10 @@
         <v>174</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G85" s="1">
         <v>1</v>
@@ -66528,10 +66560,10 @@
         <v>174</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G86" s="1">
         <v>1</v>
@@ -66545,13 +66577,13 @@
         <v>5</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G87" s="1">
         <v>1</v>
@@ -66565,73 +66597,69 @@
         <v>6</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G88" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>344</v>
-      </c>
+      <c r="A89" s="11" t="s">
+        <v>505</v>
+      </c>
+      <c r="B89" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C89" s="12"/>
+      <c r="D89" s="12" t="s">
+        <v>504</v>
+      </c>
+      <c r="E89" s="12"/>
       <c r="G89" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A90" s="8" t="s">
+      <c r="A90" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G90" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
-        <v>79</v>
+      <c r="A91" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>398</v>
+        <v>383</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>400</v>
+        <v>341</v>
       </c>
       <c r="G91" s="1">
         <v>1</v>
@@ -66642,16 +66670,16 @@
         <v>79</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="G92" s="1">
         <v>1</v>
@@ -66659,19 +66687,19 @@
     </row>
     <row r="93" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>168</v>
+        <v>6</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>306</v>
+        <v>246</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>339</v>
+        <v>393</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>175</v>
+        <v>394</v>
       </c>
       <c r="G93" s="1">
         <v>1</v>
@@ -66679,19 +66707,19 @@
     </row>
     <row r="94" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>5</v>
+        <v>168</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>274</v>
+        <v>304</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>432</v>
+        <v>335</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>344</v>
+        <v>175</v>
       </c>
       <c r="G94" s="1">
         <v>1</v>
@@ -66702,16 +66730,16 @@
         <v>81</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G95" s="1">
         <v>1</v>
@@ -66719,19 +66747,19 @@
     </row>
     <row r="96" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>168</v>
+        <v>6</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>307</v>
+        <v>273</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>402</v>
+        <v>427</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>401</v>
+        <v>341</v>
       </c>
       <c r="G96" s="1">
         <v>1</v>
@@ -66739,19 +66767,19 @@
     </row>
     <row r="97" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>168</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>217</v>
+        <v>305</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>339</v>
+        <v>397</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>176</v>
+        <v>396</v>
       </c>
       <c r="G97" s="1">
         <v>1</v>
@@ -66759,19 +66787,19 @@
     </row>
     <row r="98" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>5</v>
+        <v>168</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>308</v>
+        <v>216</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>469</v>
+        <v>335</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>344</v>
+        <v>176</v>
       </c>
       <c r="G98" s="1">
         <v>1</v>
@@ -66782,16 +66810,16 @@
         <v>84</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>469</v>
+        <v>460</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G99" s="1">
         <v>1</v>
@@ -66799,19 +66827,19 @@
     </row>
     <row r="100" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>486</v>
+        <v>460</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>341</v>
       </c>
       <c r="G100" s="1">
         <v>1</v>
@@ -66819,19 +66847,19 @@
     </row>
     <row r="101" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>155</v>
+        <v>5</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>232</v>
+        <v>309</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>177</v>
+        <v>346</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>476</v>
       </c>
       <c r="G101" s="1">
         <v>1</v>
@@ -66839,19 +66867,19 @@
     </row>
     <row r="102" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>256</v>
+        <v>230</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>344</v>
+        <v>177</v>
       </c>
       <c r="G102" s="1">
         <v>1</v>
@@ -66862,16 +66890,16 @@
         <v>87</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G103" s="1">
         <v>1</v>
@@ -66879,19 +66907,19 @@
     </row>
     <row r="104" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>216</v>
+        <v>255</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="G104" s="1">
         <v>1</v>
@@ -66902,16 +66930,16 @@
         <v>88</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G105" s="1">
         <v>1</v>
@@ -66919,19 +66947,19 @@
     </row>
     <row r="106" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>168</v>
+        <v>6</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>309</v>
+        <v>215</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>339</v>
+        <v>401</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>178</v>
+        <v>341</v>
       </c>
       <c r="G106" s="1">
         <v>1</v>
@@ -66939,19 +66967,19 @@
     </row>
     <row r="107" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>450</v>
+        <v>89</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>5</v>
+        <v>168</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>407</v>
+        <v>335</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>344</v>
+        <v>178</v>
       </c>
       <c r="G107" s="1">
         <v>1</v>
@@ -66959,19 +66987,19 @@
     </row>
     <row r="108" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>90</v>
+        <v>443</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>212</v>
+        <v>308</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>193</v>
+        <v>402</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G108" s="1">
         <v>1</v>
@@ -66979,73 +67007,75 @@
     </row>
     <row r="109" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>251</v>
+        <v>211</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>408</v>
+        <v>192</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="G109" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>345</v>
-      </c>
+      <c r="A110" s="11" t="s">
+        <v>503</v>
+      </c>
+      <c r="B110" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C110" s="12"/>
+      <c r="D110" s="12" t="s">
+        <v>506</v>
+      </c>
+      <c r="E110" s="12"/>
       <c r="G110" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A111" s="6" t="s">
-        <v>92</v>
+    <row r="111" spans="1:7" s="1" customFormat="1" ht="40" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>503</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>5</v>
+        <v>168</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>508</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>344</v>
+        <v>335</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>507</v>
       </c>
       <c r="G111" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A112" s="6" t="s">
-        <v>92</v>
+      <c r="A112" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>249</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G112" s="1">
         <v>1</v>
@@ -67053,59 +67083,53 @@
     </row>
     <row r="113" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>168</v>
+        <v>6</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>339</v>
+        <v>403</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>179</v>
+        <v>341</v>
       </c>
       <c r="G113" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
-        <v>94</v>
+      <c r="A114" s="6" t="s">
+        <v>92</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C114" s="1" t="s">
-        <v>218</v>
-      </c>
       <c r="D114" s="1" t="s">
-        <v>180</v>
+        <v>404</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G114" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
-        <v>94</v>
+      <c r="A115" s="6" t="s">
+        <v>92</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C115" s="1" t="s">
-        <v>218</v>
-      </c>
       <c r="D115" s="1" t="s">
-        <v>180</v>
+        <v>404</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G115" s="1">
         <v>1</v>
@@ -67113,19 +67137,19 @@
     </row>
     <row r="116" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>168</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>313</v>
+        <v>240</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>28</v>
+        <v>179</v>
       </c>
       <c r="G116" s="1">
         <v>1</v>
@@ -67133,19 +67157,19 @@
     </row>
     <row r="117" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>168</v>
+        <v>5</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>264</v>
+        <v>217</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>339</v>
+        <v>180</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>471</v>
+        <v>340</v>
       </c>
       <c r="G117" s="1">
         <v>1</v>
@@ -67153,19 +67177,19 @@
     </row>
     <row r="118" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>31</v>
+        <v>94</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>168</v>
+        <v>6</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>315</v>
+        <v>217</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>339</v>
+        <v>180</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>181</v>
+        <v>341</v>
       </c>
       <c r="G118" s="1">
         <v>1</v>
@@ -67173,19 +67197,19 @@
     </row>
     <row r="119" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>168</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>410</v>
+        <v>335</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>412</v>
+        <v>28</v>
       </c>
       <c r="G119" s="1">
         <v>1</v>
@@ -67193,19 +67217,19 @@
     </row>
     <row r="120" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>5</v>
+        <v>168</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>316</v>
+        <v>262</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>413</v>
+        <v>335</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>344</v>
+        <v>462</v>
       </c>
       <c r="G120" s="1">
         <v>1</v>
@@ -67213,19 +67237,19 @@
     </row>
     <row r="121" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>98</v>
+        <v>31</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>6</v>
+        <v>168</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="E121" s="2" t="s">
-        <v>345</v>
+        <v>335</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="G121" s="1">
         <v>1</v>
@@ -67233,19 +67257,19 @@
     </row>
     <row r="122" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>5</v>
+        <v>168</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>231</v>
+        <v>310</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>344</v>
+        <v>407</v>
       </c>
       <c r="G122" s="1">
         <v>1</v>
@@ -67253,19 +67277,19 @@
     </row>
     <row r="123" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>231</v>
+        <v>314</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G123" s="1">
         <v>1</v>
@@ -67273,19 +67297,19 @@
     </row>
     <row r="124" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>247</v>
+        <v>314</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>344</v>
+        <v>408</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>341</v>
       </c>
       <c r="G124" s="1">
         <v>1</v>
@@ -67293,19 +67317,19 @@
     </row>
     <row r="125" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G125" s="1">
         <v>1</v>
@@ -67313,19 +67337,19 @@
     </row>
     <row r="126" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>168</v>
+        <v>6</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>416</v>
+        <v>341</v>
       </c>
       <c r="G126" s="1">
         <v>1</v>
@@ -67333,19 +67357,19 @@
     </row>
     <row r="127" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>317</v>
+        <v>245</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E127" s="2" t="s">
-        <v>479</v>
+        <v>410</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>340</v>
       </c>
       <c r="G127" s="1">
         <v>1</v>
@@ -67353,19 +67377,19 @@
     </row>
     <row r="128" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>314</v>
+        <v>245</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="G128" s="1">
         <v>1</v>
@@ -67373,19 +67397,19 @@
     </row>
     <row r="129" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>5</v>
+        <v>168</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>182</v>
+        <v>398</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>344</v>
+        <v>411</v>
       </c>
       <c r="G129" s="1">
         <v>1</v>
@@ -67393,19 +67417,19 @@
     </row>
     <row r="130" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>243</v>
+        <v>315</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E130" s="1" t="s">
-        <v>345</v>
+        <v>193</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>469</v>
       </c>
       <c r="G130" s="1">
         <v>1</v>
@@ -67413,19 +67437,19 @@
     </row>
     <row r="131" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>168</v>
+        <v>5</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>393</v>
+        <v>312</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>339</v>
+        <v>412</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>472</v>
+        <v>340</v>
       </c>
       <c r="G131" s="1">
         <v>1</v>
@@ -67433,19 +67457,19 @@
     </row>
     <row r="132" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>268</v>
+        <v>241</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>418</v>
+        <v>182</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G132" s="1">
         <v>1</v>
@@ -67453,19 +67477,19 @@
     </row>
     <row r="133" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>269</v>
+        <v>241</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>418</v>
+        <v>182</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G133" s="1">
         <v>1</v>
@@ -67473,19 +67497,19 @@
     </row>
     <row r="134" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>5</v>
+        <v>168</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>254</v>
+        <v>388</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>419</v>
+        <v>335</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>344</v>
+        <v>463</v>
       </c>
       <c r="G134" s="1">
         <v>1</v>
@@ -67493,19 +67517,19 @@
     </row>
     <row r="135" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G135" s="1">
         <v>1</v>
@@ -67513,19 +67537,19 @@
     </row>
     <row r="136" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>421</v>
+        <v>267</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="G136" s="1">
         <v>1</v>
@@ -67533,19 +67557,19 @@
     </row>
     <row r="137" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>421</v>
+        <v>252</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G137" s="1">
         <v>1</v>
@@ -67553,19 +67577,19 @@
     </row>
     <row r="138" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>230</v>
+        <v>252</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>350</v>
+        <v>414</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>364</v>
+        <v>341</v>
       </c>
       <c r="G138" s="1">
         <v>1</v>
@@ -67573,19 +67597,19 @@
     </row>
     <row r="139" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>229</v>
+        <v>416</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>195</v>
+        <v>415</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>478</v>
+        <v>340</v>
       </c>
       <c r="G139" s="1">
         <v>1</v>
@@ -67593,19 +67617,19 @@
     </row>
     <row r="140" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>168</v>
+        <v>6</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>321</v>
+        <v>416</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>183</v>
+        <v>415</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>196</v>
+        <v>341</v>
       </c>
       <c r="G140" s="1">
         <v>1</v>
@@ -67613,19 +67637,19 @@
     </row>
     <row r="141" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C141" s="1" t="s">
-        <v>267</v>
+      <c r="C141" s="5" t="s">
+        <v>494</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>422</v>
+        <v>346</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>344</v>
+        <v>360</v>
       </c>
       <c r="G141" s="1">
         <v>1</v>
@@ -67633,39 +67657,39 @@
     </row>
     <row r="142" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>267</v>
+        <v>228</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>422</v>
+        <v>194</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>345</v>
+        <v>468</v>
       </c>
       <c r="G142" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>41</v>
+        <v>111</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>168</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>423</v>
+        <v>183</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="G143" s="1">
         <v>1</v>
@@ -67673,19 +67697,19 @@
     </row>
     <row r="144" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>348</v>
+        <v>417</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G144" s="1">
         <v>1</v>
@@ -67693,19 +67717,19 @@
     </row>
     <row r="145" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>336</v>
+        <v>265</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>348</v>
+        <v>417</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G145" s="1">
         <v>1</v>
@@ -67713,19 +67737,19 @@
     </row>
     <row r="146" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>6</v>
+        <v>168</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>239</v>
+        <v>316</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>345</v>
+        <v>184</v>
       </c>
       <c r="G146" s="1">
         <v>1</v>
@@ -67733,19 +67757,19 @@
     </row>
     <row r="147" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>168</v>
+        <v>5</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>320</v>
+        <v>268</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G147" s="1">
         <v>1</v>
@@ -67753,19 +67777,19 @@
     </row>
     <row r="148" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>319</v>
+        <v>332</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>425</v>
+        <v>344</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="G148" s="1">
         <v>1</v>
@@ -67773,19 +67797,19 @@
     </row>
     <row r="149" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>319</v>
+        <v>237</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G149" s="1">
         <v>1</v>
@@ -67793,16 +67817,19 @@
     </row>
     <row r="150" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>5</v>
+        <v>168</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>318</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>426</v>
+        <v>335</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G150" s="1">
         <v>1</v>
@@ -67810,16 +67837,19 @@
     </row>
     <row r="151" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>317</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G151" s="1">
         <v>1</v>
@@ -67827,79 +67857,73 @@
     </row>
     <row r="152" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>39</v>
+        <v>116</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D152" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="E152" s="2" t="s">
-        <v>484</v>
+        <v>317</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>341</v>
       </c>
       <c r="G152" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A153" s="2" t="s">
-        <v>118</v>
+      <c r="A153" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C153" s="1" t="s">
-        <v>322</v>
+        <v>5</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E153" s="2" t="s">
-        <v>485</v>
+        <v>421</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>340</v>
       </c>
       <c r="G153" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A154" s="2" t="s">
-        <v>119</v>
+      <c r="A154" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C154" s="1" t="s">
-        <v>257</v>
-      </c>
       <c r="D154" s="1" t="s">
-        <v>339</v>
+        <v>421</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G154" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>123</v>
+        <v>39</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>168</v>
+        <v>6</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="E155" s="1" t="s">
-        <v>185</v>
+        <v>247</v>
+      </c>
+      <c r="D155" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="E155" s="2" t="s">
+        <v>474</v>
       </c>
       <c r="G155" s="1">
         <v>1</v>
@@ -67907,19 +67931,19 @@
     </row>
     <row r="156" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>168</v>
+        <v>6</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>339</v>
+        <v>196</v>
       </c>
       <c r="E156" s="2" t="s">
-        <v>428</v>
+        <v>475</v>
       </c>
       <c r="G156" s="1">
         <v>1</v>
@@ -67927,39 +67951,39 @@
     </row>
     <row r="157" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>168</v>
+        <v>6</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>392</v>
+        <v>255</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>186</v>
+        <v>341</v>
       </c>
       <c r="G157" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="158" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>168</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G158" s="1">
         <v>1</v>
@@ -67967,19 +67991,19 @@
     </row>
     <row r="159" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>168</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>394</v>
+        <v>321</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="E159" s="1" t="s">
-        <v>473</v>
+        <v>335</v>
+      </c>
+      <c r="E159" s="2" t="s">
+        <v>423</v>
       </c>
       <c r="G159" s="1">
         <v>1</v>
@@ -67987,19 +68011,19 @@
     </row>
     <row r="160" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>5</v>
+        <v>168</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>326</v>
+        <v>387</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>431</v>
+        <v>335</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>344</v>
+        <v>186</v>
       </c>
       <c r="G160" s="1">
         <v>1</v>
@@ -68007,19 +68031,19 @@
     </row>
     <row r="161" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C161" s="1" t="s">
-        <v>326</v>
+        <v>168</v>
+      </c>
+      <c r="C161" s="5" t="s">
+        <v>495</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>431</v>
+        <v>335</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>345</v>
+        <v>187</v>
       </c>
       <c r="G161" s="1">
         <v>1</v>
@@ -68027,19 +68051,19 @@
     </row>
     <row r="162" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>5</v>
+        <v>168</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>250</v>
+        <v>389</v>
       </c>
       <c r="D162" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="E162" s="1" t="s">
         <v>464</v>
-      </c>
-      <c r="E162" s="1" t="s">
-        <v>344</v>
       </c>
       <c r="G162" s="1">
         <v>1</v>
@@ -68047,19 +68071,19 @@
     </row>
     <row r="163" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>250</v>
+        <v>323</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>464</v>
+        <v>426</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G163" s="1">
         <v>1</v>
@@ -68067,19 +68091,19 @@
     </row>
     <row r="164" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>463</v>
+        <v>426</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="G164" s="1">
         <v>1</v>
@@ -68087,19 +68111,19 @@
     </row>
     <row r="165" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>330</v>
+        <v>248</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G165" s="1">
         <v>1</v>
@@ -68107,19 +68131,19 @@
     </row>
     <row r="166" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>433</v>
+        <v>455</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="G166" s="1">
         <v>1</v>
@@ -68127,19 +68151,19 @@
     </row>
     <row r="167" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>261</v>
+        <v>325</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>433</v>
+        <v>454</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G167" s="1">
         <v>1</v>
@@ -68147,19 +68171,19 @@
     </row>
     <row r="168" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>168</v>
+        <v>6</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>430</v>
+        <v>454</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>429</v>
+        <v>341</v>
       </c>
       <c r="G168" s="1">
         <v>1</v>
@@ -68167,19 +68191,19 @@
     </row>
     <row r="169" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>258</v>
+        <v>236</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>188</v>
+        <v>428</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G169" s="1">
         <v>1</v>
@@ -68187,19 +68211,19 @@
     </row>
     <row r="170" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>225</v>
+        <v>259</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>189</v>
+        <v>428</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G170" s="1">
         <v>1</v>
@@ -68207,19 +68231,19 @@
     </row>
     <row r="171" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>6</v>
+        <v>168</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>246</v>
+        <v>324</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>190</v>
+        <v>425</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>344</v>
+        <v>424</v>
       </c>
       <c r="G171" s="1">
         <v>1</v>
@@ -68227,19 +68251,19 @@
     </row>
     <row r="172" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>168</v>
+        <v>6</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="D172" s="1" t="s">
-        <v>339</v>
+        <v>256</v>
+      </c>
+      <c r="D172" s="5" t="s">
+        <v>496</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>434</v>
+        <v>341</v>
       </c>
       <c r="G172" s="1">
         <v>1</v>
@@ -68247,19 +68271,19 @@
     </row>
     <row r="173" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>168</v>
+        <v>5</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>263</v>
+        <v>224</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="E173" s="1" t="s">
-        <v>435</v>
+        <v>188</v>
+      </c>
+      <c r="E173" s="5" t="s">
+        <v>340</v>
       </c>
       <c r="G173" s="1">
         <v>1</v>
@@ -68267,19 +68291,19 @@
     </row>
     <row r="174" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>168</v>
+        <v>6</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="E174" s="1" t="s">
-        <v>436</v>
+        <v>189</v>
+      </c>
+      <c r="E174" s="5" t="s">
+        <v>341</v>
       </c>
       <c r="G174" s="1">
         <v>1</v>
@@ -68287,19 +68311,19 @@
     </row>
     <row r="175" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>168</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>437</v>
+        <v>335</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="G175" s="1">
         <v>1</v>
@@ -68307,19 +68331,19 @@
     </row>
     <row r="176" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>440</v>
+        <v>133</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>5</v>
+        <v>168</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>441</v>
+        <v>261</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>442</v>
+        <v>335</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>344</v>
+        <v>430</v>
       </c>
       <c r="G176" s="1">
         <v>1</v>
@@ -68327,33 +68351,39 @@
     </row>
     <row r="177" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>440</v>
+        <v>134</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>6</v>
+        <v>168</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>441</v>
+        <v>231</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>442</v>
+        <v>335</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>345</v>
+        <v>431</v>
       </c>
       <c r="G177" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="178" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A178" s="1" t="s">
-        <v>44</v>
+      <c r="A178" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>46</v>
+        <v>168</v>
+      </c>
+      <c r="C178" s="5" t="s">
+        <v>498</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>432</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>191</v>
+        <v>433</v>
       </c>
       <c r="G178" s="1">
         <v>1</v>
@@ -68361,19 +68391,19 @@
     </row>
     <row r="179" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>136</v>
+        <v>435</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>334</v>
+        <v>436</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G179" s="1">
         <v>1</v>
@@ -68381,39 +68411,33 @@
     </row>
     <row r="180" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>136</v>
+        <v>435</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>334</v>
+        <v>436</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G180" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="181" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A181" s="2" t="s">
-        <v>137</v>
+      <c r="A181" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C181" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="D181" s="1" t="s">
-        <v>443</v>
+        <v>46</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>344</v>
+        <v>190</v>
       </c>
       <c r="G181" s="1">
         <v>1</v>
@@ -68421,19 +68445,19 @@
     </row>
     <row r="182" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>395</v>
+        <v>330</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G182" s="1">
         <v>1</v>
@@ -68441,39 +68465,39 @@
     </row>
     <row r="183" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>265</v>
+        <v>330</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>198</v>
+        <v>434</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>491</v>
+        <v>341</v>
       </c>
       <c r="G183" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="184" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A184" s="6" t="s">
-        <v>139</v>
+      <c r="A184" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C184" s="4" t="s">
-        <v>331</v>
+      <c r="C184" s="1" t="s">
+        <v>390</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G184" s="1">
         <v>1</v>
@@ -68481,59 +68505,59 @@
     </row>
     <row r="185" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C185" s="4" t="s">
-        <v>331</v>
+      <c r="C185" s="1" t="s">
+        <v>390</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G185" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="186" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A186" s="5" t="s">
-        <v>382</v>
+      <c r="A186" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>383</v>
+        <v>263</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>151</v>
+        <v>197</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>344</v>
+        <v>481</v>
       </c>
       <c r="G186" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="187" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A187" s="1" t="s">
-        <v>382</v>
+      <c r="A187" s="6" t="s">
+        <v>139</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C187" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="D187" s="1" t="s">
-        <v>151</v>
+        <v>5</v>
+      </c>
+      <c r="C187" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="D187" s="5" t="s">
+        <v>499</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G187" s="1">
         <v>1</v>
@@ -68541,59 +68565,59 @@
     </row>
     <row r="188" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C188" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="D188" s="1" t="s">
-        <v>339</v>
+        <v>6</v>
+      </c>
+      <c r="C188" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="D188" s="5" t="s">
+        <v>499</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>445</v>
+        <v>341</v>
       </c>
       <c r="G188" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="189" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A189" s="2" t="s">
-        <v>141</v>
+      <c r="A189" s="9" t="s">
+        <v>377</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>397</v>
+        <v>378</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>447</v>
+        <v>151</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G189" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="190" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A190" s="2" t="s">
-        <v>142</v>
+      <c r="A190" s="1" t="s">
+        <v>377</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>278</v>
+        <v>378</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>466</v>
+        <v>151</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="G190" s="1">
         <v>1</v>
@@ -68601,19 +68625,19 @@
     </row>
     <row r="191" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>6</v>
+        <v>168</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>279</v>
+        <v>391</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>466</v>
+        <v>335</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>345</v>
+        <v>439</v>
       </c>
       <c r="G191" s="1">
         <v>1</v>
@@ -68621,19 +68645,19 @@
     </row>
     <row r="192" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>266</v>
+        <v>392</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G192" s="1">
         <v>1</v>
@@ -68641,19 +68665,19 @@
     </row>
     <row r="193" spans="1:8" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>448</v>
+        <v>457</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G193" s="1">
         <v>1</v>
@@ -68661,19 +68685,19 @@
     </row>
     <row r="194" spans="1:8" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>168</v>
+        <v>6</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>333</v>
+        <v>277</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>339</v>
+        <v>457</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>200</v>
+        <v>341</v>
       </c>
       <c r="G194" s="1">
         <v>1</v>
@@ -68681,19 +68705,19 @@
     </row>
     <row r="195" spans="1:8" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>168</v>
+        <v>5</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="D195" s="1" t="s">
-        <v>391</v>
+        <v>264</v>
+      </c>
+      <c r="D195" s="5" t="s">
+        <v>500</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>474</v>
+        <v>340</v>
       </c>
       <c r="G195" s="1">
         <v>1</v>
@@ -68701,19 +68725,19 @@
     </row>
     <row r="196" spans="1:8" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D196" s="1" t="s">
-        <v>201</v>
+        <v>264</v>
+      </c>
+      <c r="D196" s="5" t="s">
+        <v>500</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="G196" s="1">
         <v>1</v>
@@ -68721,19 +68745,19 @@
     </row>
     <row r="197" spans="1:8" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>6</v>
+        <v>168</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>280</v>
+        <v>329</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>201</v>
+        <v>335</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>345</v>
+        <v>199</v>
       </c>
       <c r="G197" s="1">
         <v>1</v>
@@ -68741,19 +68765,19 @@
     </row>
     <row r="198" spans="1:8" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>5</v>
+        <v>168</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="D198" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="E198" s="1" t="s">
-        <v>344</v>
+        <v>279</v>
+      </c>
+      <c r="D198" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="E198" s="5" t="s">
+        <v>501</v>
       </c>
       <c r="G198" s="1">
         <v>1</v>
@@ -68761,19 +68785,19 @@
     </row>
     <row r="199" spans="1:8" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>259</v>
+        <v>278</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>449</v>
+        <v>200</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G199" s="1">
         <v>1</v>
@@ -68781,19 +68805,19 @@
     </row>
     <row r="200" spans="1:8" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>168</v>
+        <v>6</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>339</v>
+        <v>200</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>470</v>
+        <v>341</v>
       </c>
       <c r="G200" s="1">
         <v>1</v>
@@ -68801,19 +68825,19 @@
     </row>
     <row r="201" spans="1:8" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>227</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G201" s="1">
         <v>1</v>
@@ -68821,112 +68845,172 @@
     </row>
     <row r="202" spans="1:8" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>452</v>
+        <v>147</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>460</v>
+        <v>257</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>457</v>
+        <v>442</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="F202"/>
+        <v>341</v>
+      </c>
       <c r="G202" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="203" spans="1:8" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>453</v>
+        <v>148</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>6</v>
+        <v>168</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>459</v>
+        <v>269</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>458</v>
+        <v>335</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="F203"/>
+        <v>461</v>
+      </c>
       <c r="G203" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="204" spans="1:8" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A204" s="7" t="s">
-        <v>150</v>
+      <c r="A204" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>161</v>
+        <v>6</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>337</v>
+        <v>226</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>335</v>
+        <v>444</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>455</v>
+        <v>341</v>
       </c>
       <c r="G204" s="1">
         <v>1</v>
       </c>
-      <c r="H204"/>
     </row>
     <row r="205" spans="1:8" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C205" s="10" t="s">
-        <v>502</v>
+        <v>5</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>453</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>461</v>
+        <v>450</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>462</v>
+        <v>340</v>
       </c>
       <c r="F205"/>
       <c r="G205" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>207</v>
+        <v>446</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>155</v>
+        <v>6</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>226</v>
+        <v>452</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="F206" s="1"/>
+        <v>341</v>
+      </c>
+      <c r="F206"/>
       <c r="G206" s="1">
         <v>1</v>
       </c>
     </row>
+    <row r="207" spans="1:8" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A207" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D207" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E207" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="G207" s="1">
+        <v>1</v>
+      </c>
+      <c r="H207"/>
+    </row>
+    <row r="208" spans="1:8" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A208" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C208" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="D208" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="E208" s="5" t="s">
+        <v>502</v>
+      </c>
+      <c r="F208"/>
+      <c r="G208" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A209" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="E209" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="F209" s="1"/>
+      <c r="G209" s="1">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G206">
-    <sortCondition ref="A2:A206"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G209">
+    <sortCondition ref="A2:A209"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Edits to card data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleylucouch/Documents/TRAAB_Cards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376D8C88-77BA-1D4C-BFA8-DFFCB79D090D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9087183B-0687-3A4D-93CE-D7222F6F0C9C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19200" xr2:uid="{D5C866A4-9C33-EB4E-9D4B-68221F48654F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="510">
   <si>
     <t>AGORAPHOBE</t>
   </si>
@@ -502,9 +502,6 @@
   </si>
   <si>
     <t>So many legs!</t>
-  </si>
-  <si>
-    <t>I will turn you</t>
   </si>
   <si>
     <t>It is what I do best</t>
@@ -1188,12 +1185,6 @@
     <t>Any player that card shares or color shares with you immediately trades cards with you. You both assume the powers and the allegiance of the newly acquired cards.</t>
   </si>
   <si>
-    <t>If you are in the same room as the President and Bomber at the end of the game, you win.</t>
-  </si>
-  <si>
-    <t>If you win, both the Red Team and Blue Team lose.</t>
-  </si>
-  <si>
     <t>A solid choice</t>
   </si>
   <si>
@@ -1245,9 +1236,6 @@
     <t>When you publicly reveal your card, your vote counts as two votes. This means that you can publicly reveal your card to count as two people for or against the nomination of a new leader.</t>
   </si>
   <si>
-    <t>Any player that card shares with you has all conditions removed.</t>
-  </si>
-  <si>
     <t>During the first round you must privately reveal your card to 2 players and verbally say to them: "You are my children."</t>
   </si>
   <si>
@@ -1294,9 +1282,6 @@
   </si>
   <si>
     <t>If you 1) are a room’s leader, 2) have selected hostages, 3) are between rounds, and 4) are waiting for the other room’s leader, you may yell "I’m a raging one! I’m a raging two! ..." continuing until either the leader shows up or you say "I’m a raging ten!" If you say "I’m a raging ten!", you win and all other players lose.</t>
-  </si>
-  <si>
-    <t>Once per game, you may publicly reveal your card and go to the opposing room. There, you are immune to all powers and conditions. In the other room, Rats cannot take part in votes and can not be a hostage. If you do not return to your original room before the end of the round, you lose.</t>
   </si>
   <si>
     <t>If the first player with whom you card share or color share wins, you win. If you fail to color share or card share with any other player, you lose.</t>
@@ -1521,19 +1506,7 @@
     <t>Thus with a kiss I die</t>
   </si>
   <si>
-    <t>Any player that card shares with you must trade in their character card for a Red Team card before the beginning of the next round and before revealing any part of their card to another player. (Your power has no effect on primary characters, backup characters, or non- Red/Blue Characters.)</t>
-  </si>
-  <si>
-    <t>Any player that card shares with you must trade in their character card for a Blue Team card before the beginning of the next round and before revealing any part of their card to another player. (Your power has no effect on primary characters, backup characters, or non- Red/Blue Characters.)</t>
-  </si>
-  <si>
     <t>I know what you're planning</t>
-  </si>
-  <si>
-    <t>You have the "trade" power: you may trade your card for the buried card. You may not peek at the buried card, only trade with it, and you assume all powers and the allegiance of your newly acquired card. The "trade" power can be used by the Trader once per round.</t>
-  </si>
-  <si>
-    <t>You have the "seductive" power: any player who card shares with you that has a color not of your own gains the "seduced" condition: "seduced" players must do anything with their card that you ask of them and must vote for or against leaders as you do.</t>
   </si>
   <si>
     <t>If, at the end of the game, you are in the same room as the President, but opposite room as the Bomber, you win. If you win, both the Red and Blue Team lose.</t>
@@ -1558,6 +1531,36 @@
   </si>
   <si>
     <t>You've fallen into my trap</t>
+  </si>
+  <si>
+    <t>You have the "trade" power: you may trade your card for the buried card. You may not peek at the buried card, only trade with it, and you assume all powers and the allegiance of your newly acquired card. The "trade" power can be used once per round, even if the buried card is another Trader card.</t>
+  </si>
+  <si>
+    <t>Any player who card shares with you that has a color not of your own gains the "seduced" condition: "seduced" players must do anything with their card that you ask of them and must vote for or against leaders as you do.</t>
+  </si>
+  <si>
+    <t>If you are in the same room as the President and Bomber at the end of the game, you win. If you win, both the Red Team and Blue Team lose.</t>
+  </si>
+  <si>
+    <t>Any player that card shares with you must trade their character card for a Blue Team card before the beginning of the next round and before revealing any part of their card to another player (this power has no effect on primary characters, their backups, or characters not aligned with either Red or Blue).</t>
+  </si>
+  <si>
+    <t>Any player that card shares with you must trade their character card for a Red Team card before the beginning of the next round and before revealing any part of their card to another player (this power has no effect on primary characters, their backups, or characters not aligned with either Red or Blue).</t>
+  </si>
+  <si>
+    <t>Any player that card shares with you has all of their conditions removed.</t>
+  </si>
+  <si>
+    <t>Where does it hurt?</t>
+  </si>
+  <si>
+    <t>Once per game, you may publicly reveal your card and go to the opposing room. There, you are immune to all powers and conditions. In the other room, you cannot take part in votes and cannot be a hostage. If you do not return to your original room before the end of the round, you lose.</t>
+  </si>
+  <si>
+    <t>Squeak Squeak</t>
+  </si>
+  <si>
+    <t>Work with me</t>
   </si>
 </sst>
 </file>
@@ -1588,30 +1591,23 @@
     </font>
     <font>
       <sz val="14"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1622,12 +1618,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1650,7 +1640,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1658,14 +1648,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1983,9 +1972,9 @@
   <dimension ref="A1:WHQ209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="D106" sqref="D106"/>
+      <selection pane="bottomLeft" activeCell="G141" sqref="G141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1999,25 +1988,25 @@
   <sheetData>
     <row r="1" spans="1:15773" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>166</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:15773" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -2028,13 +2017,13 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G2" s="1">
         <v>1</v>
@@ -2048,13 +2037,13 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
@@ -2065,16 +2054,16 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>335</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>336</v>
       </c>
       <c r="G4" s="1">
         <v>1</v>
@@ -2085,13 +2074,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>1</v>
@@ -2111,13 +2100,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="G6" s="1">
         <v>1</v>
@@ -64959,13 +64948,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
@@ -64979,13 +64968,13 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
@@ -64999,13 +64988,13 @@
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G9" s="1">
         <v>1</v>
@@ -65019,13 +65008,13 @@
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G10" s="1">
         <v>1</v>
@@ -65039,13 +65028,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>32</v>
@@ -65059,16 +65048,16 @@
         <v>43</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G12" s="1">
         <v>1</v>
@@ -65085,10 +65074,10 @@
         <v>34</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G13" s="1">
         <v>1</v>
@@ -65105,10 +65094,10 @@
         <v>34</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G14" s="1">
         <v>1</v>
@@ -65122,13 +65111,13 @@
         <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="G15" s="1">
         <v>1</v>
@@ -65142,13 +65131,13 @@
         <v>155</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G16" s="1">
         <v>1</v>
@@ -65162,13 +65151,13 @@
         <v>5</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G17" s="1">
         <v>1</v>
@@ -65182,13 +65171,13 @@
         <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G18" s="1">
         <v>1</v>
@@ -65202,13 +65191,13 @@
         <v>5</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>39</v>
@@ -65225,13 +65214,13 @@
         <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="G20" s="1">
         <v>1</v>
@@ -65239,19 +65228,19 @@
     </row>
     <row r="21" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G21" s="1">
         <v>10</v>
@@ -65268,10 +65257,10 @@
         <v>35</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G22" s="1">
         <v>1</v>
@@ -65288,10 +65277,10 @@
         <v>35</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G23" s="1">
         <v>1</v>
@@ -65305,13 +65294,13 @@
         <v>6</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G24" s="1">
         <v>2</v>
@@ -65322,13 +65311,13 @@
         <v>14</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>152</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>36</v>
@@ -65345,13 +65334,13 @@
         <v>5</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>37</v>
@@ -65368,13 +65357,13 @@
         <v>6</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>37</v>
@@ -65391,13 +65380,13 @@
         <v>5</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>153</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G28" s="1">
         <v>1</v>
@@ -65411,13 +65400,13 @@
         <v>6</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>153</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G29" s="1">
         <v>1</v>
@@ -65428,13 +65417,13 @@
         <v>48</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>154</v>
@@ -65451,13 +65440,13 @@
         <v>5</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>497</v>
+        <v>234</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>503</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G31" s="1">
         <v>1</v>
@@ -65474,10 +65463,10 @@
         <v>156</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G32" s="1">
         <v>1</v>
@@ -65494,10 +65483,10 @@
         <v>156</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G33" s="1">
         <v>1</v>
@@ -65508,16 +65497,16 @@
         <v>18</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G34" s="1">
         <v>1</v>
@@ -65525,19 +65514,19 @@
     </row>
     <row r="35" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G35" s="1">
         <v>1</v>
@@ -65545,19 +65534,19 @@
     </row>
     <row r="36" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G36" s="1">
         <v>1</v>
@@ -65565,19 +65554,19 @@
     </row>
     <row r="37" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="G37" s="1">
         <v>1</v>
@@ -65585,19 +65574,19 @@
     </row>
     <row r="38" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G38" s="1">
         <v>1</v>
@@ -65605,19 +65594,19 @@
     </row>
     <row r="39" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G39" s="1">
         <v>1</v>
@@ -65631,13 +65620,13 @@
         <v>5</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>157</v>
+        <v>509</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G40" s="1">
         <v>1</v>
@@ -65651,13 +65640,13 @@
         <v>6</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>157</v>
+        <v>509</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G41" s="1">
         <v>1</v>
@@ -65671,13 +65660,13 @@
         <v>5</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G42" s="1">
         <v>1</v>
@@ -65691,13 +65680,13 @@
         <v>6</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G43" s="1">
         <v>1</v>
@@ -65711,13 +65700,13 @@
         <v>5</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G44" s="1">
         <v>1</v>
@@ -65731,13 +65720,13 @@
         <v>6</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G45" s="1">
         <v>1</v>
@@ -65748,16 +65737,16 @@
         <v>54</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D46" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>358</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>359</v>
       </c>
       <c r="G46" s="1">
         <v>1</v>
@@ -65771,13 +65760,13 @@
         <v>6</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G47" s="1">
         <v>1</v>
@@ -65791,13 +65780,13 @@
         <v>5</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G48" s="1">
         <v>1</v>
@@ -65811,13 +65800,13 @@
         <v>6</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G49" s="1">
         <v>1</v>
@@ -65828,16 +65817,16 @@
         <v>20</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>38</v>
@@ -65854,13 +65843,13 @@
         <v>5</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G51" s="1">
         <v>1</v>
@@ -65874,13 +65863,13 @@
         <v>6</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G52" s="1">
         <v>1</v>
@@ -65894,13 +65883,13 @@
         <v>5</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="G53" s="1">
         <v>1</v>
@@ -65914,13 +65903,13 @@
         <v>6</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G54" s="1">
         <v>1</v>
@@ -65934,13 +65923,13 @@
         <v>6</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="G55" s="1">
         <v>1</v>
@@ -65954,13 +65943,13 @@
         <v>6</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="G56" s="1">
         <v>1</v>
@@ -65974,13 +65963,13 @@
         <v>8</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G57" s="1">
         <v>1</v>
@@ -65991,16 +65980,16 @@
         <v>56</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="D58" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G58" s="1">
         <v>1</v>
@@ -66014,13 +66003,13 @@
         <v>6</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="G59" s="1">
         <v>1</v>
@@ -66034,13 +66023,13 @@
         <v>5</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G60" s="1">
         <v>1</v>
@@ -66054,13 +66043,13 @@
         <v>6</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G61" s="1">
         <v>1</v>
@@ -66070,17 +66059,17 @@
       <c r="A62" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="G62" s="1">
         <v>1</v>
@@ -66094,13 +66083,13 @@
         <v>5</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>340</v>
+        <v>454</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>339</v>
       </c>
       <c r="G63" s="1">
         <v>1</v>
@@ -66114,13 +66103,13 @@
         <v>6</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G64" s="1">
         <v>1</v>
@@ -66134,13 +66123,13 @@
         <v>5</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G65" s="1">
         <v>1</v>
@@ -66154,13 +66143,13 @@
         <v>5</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>492</v>
+        <v>252</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>487</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G66" s="1">
         <v>1</v>
@@ -66174,13 +66163,13 @@
         <v>6</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>492</v>
+        <v>252</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>487</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G67" s="1">
         <v>1</v>
@@ -66194,13 +66183,13 @@
         <v>6</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>493</v>
+        <v>159</v>
+      </c>
+      <c r="E68" s="10" t="s">
+        <v>488</v>
       </c>
       <c r="G68" s="1">
         <v>1</v>
@@ -66214,13 +66203,13 @@
         <v>5</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="G69" s="1">
         <v>1</v>
@@ -66231,16 +66220,16 @@
         <v>67</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="G70" s="1">
         <v>1</v>
@@ -66254,13 +66243,13 @@
         <v>5</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G71" s="1">
         <v>1</v>
@@ -66271,16 +66260,16 @@
         <v>25</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G72" s="1">
         <v>1</v>
@@ -66294,13 +66283,13 @@
         <v>5</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G73" s="1">
         <v>1</v>
@@ -66314,13 +66303,13 @@
         <v>6</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G74" s="1">
         <v>1</v>
@@ -66331,16 +66320,16 @@
         <v>27</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>41</v>
@@ -66357,13 +66346,13 @@
         <v>6</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G76" s="1">
         <v>1</v>
@@ -66374,16 +66363,16 @@
         <v>71</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G77" s="1">
         <v>3</v>
@@ -66397,13 +66386,13 @@
         <v>5</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G78" s="1">
         <v>1</v>
@@ -66417,13 +66406,13 @@
         <v>6</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G79" s="1">
         <v>1</v>
@@ -66437,13 +66426,13 @@
         <v>5</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G80" s="1">
         <v>1</v>
@@ -66457,13 +66446,13 @@
         <v>6</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G81" s="1">
         <v>1</v>
@@ -66471,19 +66460,19 @@
     </row>
     <row r="82" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>205</v>
-      </c>
       <c r="E82" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G82" s="1">
         <v>1</v>
@@ -66494,36 +66483,36 @@
         <v>74</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>386</v>
+        <v>334</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>385</v>
+        <v>502</v>
       </c>
       <c r="G83" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A84" s="7" t="s">
+      <c r="A84" s="11" t="s">
         <v>75</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G84" s="1">
         <v>1</v>
@@ -66537,13 +66526,13 @@
         <v>5</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G85" s="1">
         <v>1</v>
@@ -66557,13 +66546,13 @@
         <v>6</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G86" s="1">
         <v>1</v>
@@ -66577,13 +66566,13 @@
         <v>5</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G87" s="1">
         <v>1</v>
@@ -66597,32 +66586,32 @@
         <v>6</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G88" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A89" s="11" t="s">
-        <v>505</v>
-      </c>
-      <c r="B89" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C89" s="12"/>
-      <c r="D89" s="12" t="s">
-        <v>504</v>
-      </c>
-      <c r="E89" s="12"/>
+      <c r="A89" s="8" t="s">
+        <v>496</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C89" s="9"/>
+      <c r="D89" s="9" t="s">
+        <v>495</v>
+      </c>
+      <c r="E89" s="9"/>
       <c r="G89" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -66633,33 +66622,33 @@
         <v>5</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G90" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A91" s="7" t="s">
+      <c r="A91" s="11" t="s">
         <v>78</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G91" s="1">
         <v>1</v>
@@ -66673,13 +66662,13 @@
         <v>5</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="G92" s="1">
         <v>1</v>
@@ -66693,13 +66682,13 @@
         <v>6</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G93" s="1">
         <v>1</v>
@@ -66710,16 +66699,16 @@
         <v>80</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G94" s="1">
         <v>1</v>
@@ -66733,13 +66722,13 @@
         <v>5</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G95" s="1">
         <v>1</v>
@@ -66753,13 +66742,13 @@
         <v>6</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G96" s="1">
         <v>1</v>
@@ -66770,16 +66759,16 @@
         <v>82</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="G97" s="1">
         <v>1</v>
@@ -66790,16 +66779,16 @@
         <v>83</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G98" s="1">
         <v>1</v>
@@ -66813,13 +66802,13 @@
         <v>5</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G99" s="1">
         <v>1</v>
@@ -66833,13 +66822,13 @@
         <v>6</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G100" s="1">
         <v>1</v>
@@ -66853,13 +66842,13 @@
         <v>5</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="G101" s="1">
         <v>1</v>
@@ -66873,13 +66862,13 @@
         <v>155</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G102" s="1">
         <v>1</v>
@@ -66893,13 +66882,13 @@
         <v>5</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G103" s="1">
         <v>1</v>
@@ -66913,13 +66902,13 @@
         <v>6</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G104" s="1">
         <v>1</v>
@@ -66933,13 +66922,13 @@
         <v>5</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G105" s="1">
         <v>1</v>
@@ -66953,13 +66942,13 @@
         <v>6</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G106" s="1">
         <v>1</v>
@@ -66970,16 +66959,16 @@
         <v>89</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G107" s="1">
         <v>1</v>
@@ -66987,19 +66976,19 @@
     </row>
     <row r="108" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G108" s="1">
         <v>1</v>
@@ -67013,49 +67002,49 @@
         <v>6</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G109" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A110" s="11" t="s">
-        <v>503</v>
-      </c>
-      <c r="B110" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C110" s="12"/>
-      <c r="D110" s="12" t="s">
-        <v>506</v>
-      </c>
-      <c r="E110" s="12"/>
+      <c r="A110" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C110" s="9"/>
+      <c r="D110" s="9" t="s">
+        <v>497</v>
+      </c>
+      <c r="E110" s="9"/>
       <c r="G110" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:7" s="1" customFormat="1" ht="40" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>507</v>
+        <v>498</v>
       </c>
       <c r="G111" s="1">
         <v>1</v>
@@ -67069,13 +67058,13 @@
         <v>5</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G112" s="1">
         <v>1</v>
@@ -67089,47 +67078,53 @@
         <v>6</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G113" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A114" s="6" t="s">
+      <c r="A114" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C114" s="1" t="s">
+        <v>506</v>
+      </c>
       <c r="D114" s="1" t="s">
-        <v>404</v>
+        <v>505</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G114" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A115" s="6" t="s">
+      <c r="A115" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C115" s="1" t="s">
+        <v>506</v>
+      </c>
       <c r="D115" s="1" t="s">
-        <v>404</v>
+        <v>505</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G115" s="1">
         <v>1</v>
@@ -67140,16 +67135,16 @@
         <v>93</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G116" s="1">
         <v>1</v>
@@ -67163,13 +67158,13 @@
         <v>5</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G117" s="1">
         <v>1</v>
@@ -67183,13 +67178,13 @@
         <v>6</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G118" s="1">
         <v>1</v>
@@ -67200,13 +67195,13 @@
         <v>95</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>28</v>
@@ -67220,16 +67215,16 @@
         <v>96</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="G120" s="1">
         <v>1</v>
@@ -67240,16 +67235,16 @@
         <v>31</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G121" s="1">
         <v>1</v>
@@ -67260,16 +67255,16 @@
         <v>97</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="G122" s="1">
         <v>1</v>
@@ -67283,13 +67278,13 @@
         <v>5</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G123" s="1">
         <v>1</v>
@@ -67303,13 +67298,13 @@
         <v>6</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G124" s="1">
         <v>1</v>
@@ -67323,13 +67318,13 @@
         <v>5</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G125" s="1">
         <v>1</v>
@@ -67343,13 +67338,13 @@
         <v>6</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G126" s="1">
         <v>1</v>
@@ -67363,13 +67358,13 @@
         <v>5</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G127" s="1">
         <v>1</v>
@@ -67383,13 +67378,13 @@
         <v>6</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G128" s="1">
         <v>1</v>
@@ -67400,16 +67395,16 @@
         <v>101</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="G129" s="1">
         <v>1</v>
@@ -67423,13 +67418,13 @@
         <v>5</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="G130" s="1">
         <v>1</v>
@@ -67443,13 +67438,13 @@
         <v>5</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G131" s="1">
         <v>1</v>
@@ -67463,13 +67458,13 @@
         <v>5</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G132" s="1">
         <v>1</v>
@@ -67483,13 +67478,13 @@
         <v>6</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G133" s="1">
         <v>1</v>
@@ -67500,16 +67495,16 @@
         <v>105</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="G134" s="1">
         <v>1</v>
@@ -67523,13 +67518,13 @@
         <v>5</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G135" s="1">
         <v>1</v>
@@ -67543,13 +67538,13 @@
         <v>6</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G136" s="1">
         <v>1</v>
@@ -67563,13 +67558,13 @@
         <v>5</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G137" s="1">
         <v>1</v>
@@ -67583,13 +67578,13 @@
         <v>6</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G138" s="1">
         <v>1</v>
@@ -67603,13 +67598,13 @@
         <v>5</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G139" s="1">
         <v>1</v>
@@ -67623,13 +67618,13 @@
         <v>6</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G140" s="1">
         <v>1</v>
@@ -67642,17 +67637,17 @@
       <c r="B141" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C141" s="5" t="s">
-        <v>494</v>
+      <c r="C141" s="10" t="s">
+        <v>489</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G141" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -67663,16 +67658,16 @@
         <v>5</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="G142" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -67680,16 +67675,16 @@
         <v>111</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G143" s="1">
         <v>1</v>
@@ -67703,13 +67698,13 @@
         <v>5</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G144" s="1">
         <v>1</v>
@@ -67723,13 +67718,13 @@
         <v>6</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G145" s="1">
         <v>1</v>
@@ -67740,16 +67735,16 @@
         <v>41</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G146" s="1">
         <v>1</v>
@@ -67763,13 +67758,13 @@
         <v>5</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G147" s="1">
         <v>1</v>
@@ -67783,13 +67778,13 @@
         <v>6</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G148" s="1">
         <v>1</v>
@@ -67803,13 +67798,13 @@
         <v>6</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G149" s="1">
         <v>1</v>
@@ -67820,16 +67815,16 @@
         <v>115</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G150" s="1">
         <v>1</v>
@@ -67843,13 +67838,13 @@
         <v>5</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G151" s="1">
         <v>1</v>
@@ -67863,47 +67858,53 @@
         <v>6</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G152" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A153" s="6" t="s">
+      <c r="A153" s="5" t="s">
         <v>117</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C153" s="1" t="s">
+        <v>508</v>
+      </c>
       <c r="D153" s="1" t="s">
-        <v>421</v>
+        <v>507</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G153" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A154" s="6" t="s">
+      <c r="A154" s="5" t="s">
         <v>117</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C154" s="1" t="s">
+        <v>508</v>
+      </c>
       <c r="D154" s="1" t="s">
-        <v>421</v>
+        <v>507</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G154" s="1">
         <v>1</v>
@@ -67917,13 +67918,13 @@
         <v>6</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="G155" s="1">
         <v>1</v>
@@ -67937,13 +67938,13 @@
         <v>6</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E156" s="2" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="G156" s="1">
         <v>1</v>
@@ -67957,13 +67958,13 @@
         <v>6</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G157" s="1">
         <v>10</v>
@@ -67974,16 +67975,16 @@
         <v>123</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G158" s="1">
         <v>1</v>
@@ -67994,16 +67995,16 @@
         <v>120</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="G159" s="1">
         <v>1</v>
@@ -68014,16 +68015,16 @@
         <v>121</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G160" s="1">
         <v>1</v>
@@ -68034,16 +68035,16 @@
         <v>122</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C161" s="5" t="s">
-        <v>495</v>
+        <v>167</v>
+      </c>
+      <c r="C161" s="10" t="s">
+        <v>490</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G161" s="1">
         <v>1</v>
@@ -68054,16 +68055,16 @@
         <v>124</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="G162" s="1">
         <v>1</v>
@@ -68077,13 +68078,13 @@
         <v>5</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G163" s="1">
         <v>1</v>
@@ -68097,13 +68098,13 @@
         <v>6</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G164" s="1">
         <v>1</v>
@@ -68117,13 +68118,13 @@
         <v>5</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G165" s="1">
         <v>1</v>
@@ -68137,13 +68138,13 @@
         <v>6</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G166" s="1">
         <v>1</v>
@@ -68157,13 +68158,13 @@
         <v>5</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G167" s="1">
         <v>1</v>
@@ -68177,13 +68178,13 @@
         <v>6</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G168" s="1">
         <v>1</v>
@@ -68197,13 +68198,13 @@
         <v>5</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G169" s="1">
         <v>1</v>
@@ -68217,13 +68218,13 @@
         <v>6</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G170" s="1">
         <v>1</v>
@@ -68234,16 +68235,16 @@
         <v>125</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="G171" s="1">
         <v>1</v>
@@ -68257,13 +68258,13 @@
         <v>6</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="D172" s="5" t="s">
-        <v>496</v>
+        <v>255</v>
+      </c>
+      <c r="D172" s="10" t="s">
+        <v>504</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G172" s="1">
         <v>1</v>
@@ -68277,12 +68278,12 @@
         <v>5</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E173" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E173" s="1" t="s">
         <v>340</v>
       </c>
       <c r="G173" s="1">
@@ -68297,13 +68298,13 @@
         <v>6</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E174" s="5" t="s">
-        <v>341</v>
+        <v>188</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>339</v>
       </c>
       <c r="G174" s="1">
         <v>1</v>
@@ -68314,16 +68315,16 @@
         <v>132</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="G175" s="1">
         <v>1</v>
@@ -68334,16 +68335,16 @@
         <v>133</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="G176" s="1">
         <v>1</v>
@@ -68354,16 +68355,16 @@
         <v>134</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="G177" s="1">
         <v>1</v>
@@ -68374,16 +68375,16 @@
         <v>135</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C178" s="5" t="s">
-        <v>498</v>
+        <v>167</v>
+      </c>
+      <c r="C178" s="10" t="s">
+        <v>491</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="G178" s="1">
         <v>1</v>
@@ -68391,19 +68392,19 @@
     </row>
     <row r="179" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G179" s="1">
         <v>1</v>
@@ -68411,19 +68412,19 @@
     </row>
     <row r="180" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G180" s="1">
         <v>1</v>
@@ -68437,7 +68438,7 @@
         <v>46</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G181" s="1">
         <v>1</v>
@@ -68451,13 +68452,13 @@
         <v>5</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G182" s="1">
         <v>1</v>
@@ -68471,13 +68472,13 @@
         <v>6</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G183" s="1">
         <v>1</v>
@@ -68491,13 +68492,13 @@
         <v>5</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G184" s="1">
         <v>1</v>
@@ -68511,13 +68512,13 @@
         <v>6</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G185" s="1">
         <v>1</v>
@@ -68531,33 +68532,33 @@
         <v>6</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="G186" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="187" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A187" s="6" t="s">
+      <c r="A187" s="5" t="s">
         <v>139</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="D187" s="5" t="s">
-        <v>499</v>
+        <v>326</v>
+      </c>
+      <c r="D187" s="10" t="s">
+        <v>500</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G187" s="1">
         <v>1</v>
@@ -68571,33 +68572,33 @@
         <v>6</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="D188" s="5" t="s">
-        <v>499</v>
+        <v>326</v>
+      </c>
+      <c r="D188" s="10" t="s">
+        <v>500</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G188" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="189" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A189" s="9" t="s">
-        <v>377</v>
+      <c r="A189" s="7" t="s">
+        <v>376</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D189" s="1" t="s">
         <v>151</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G189" s="1">
         <v>1</v>
@@ -68605,19 +68606,19 @@
     </row>
     <row r="190" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D190" s="1" t="s">
         <v>151</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G190" s="1">
         <v>1</v>
@@ -68628,16 +68629,16 @@
         <v>140</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="G191" s="1">
         <v>1</v>
@@ -68651,13 +68652,13 @@
         <v>5</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G192" s="1">
         <v>1</v>
@@ -68671,13 +68672,13 @@
         <v>5</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G193" s="1">
         <v>1</v>
@@ -68691,13 +68692,13 @@
         <v>6</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G194" s="1">
         <v>1</v>
@@ -68711,13 +68712,13 @@
         <v>5</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="D195" s="5" t="s">
-        <v>500</v>
+        <v>263</v>
+      </c>
+      <c r="D195" s="10" t="s">
+        <v>501</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G195" s="1">
         <v>1</v>
@@ -68731,13 +68732,13 @@
         <v>6</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="D196" s="5" t="s">
-        <v>500</v>
+        <v>263</v>
+      </c>
+      <c r="D196" s="10" t="s">
+        <v>501</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G196" s="1">
         <v>1</v>
@@ -68748,16 +68749,16 @@
         <v>144</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G197" s="1">
         <v>1</v>
@@ -68768,16 +68769,16 @@
         <v>145</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="D198" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="E198" s="5" t="s">
-        <v>501</v>
+        <v>278</v>
+      </c>
+      <c r="D198" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="E198" s="10" t="s">
+        <v>492</v>
       </c>
       <c r="G198" s="1">
         <v>1</v>
@@ -68791,13 +68792,13 @@
         <v>5</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G199" s="1">
         <v>1</v>
@@ -68811,13 +68812,13 @@
         <v>6</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G200" s="1">
         <v>1</v>
@@ -68831,13 +68832,13 @@
         <v>5</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G201" s="1">
         <v>1</v>
@@ -68851,13 +68852,13 @@
         <v>6</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G202" s="1">
         <v>1</v>
@@ -68868,16 +68869,16 @@
         <v>148</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="G203" s="1">
         <v>1</v>
@@ -68891,13 +68892,13 @@
         <v>6</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G204" s="1">
         <v>1</v>
@@ -68905,19 +68906,19 @@
     </row>
     <row r="205" spans="1:8" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F205"/>
       <c r="G205" s="1">
@@ -68926,19 +68927,19 @@
     </row>
     <row r="206" spans="1:8" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F206"/>
       <c r="G206" s="1">
@@ -68950,16 +68951,16 @@
         <v>150</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="G207" s="1">
         <v>1</v>
@@ -68968,19 +68969,19 @@
     </row>
     <row r="208" spans="1:8" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C208" s="8" t="s">
-        <v>491</v>
-      </c>
-      <c r="D208" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="E208" s="5" t="s">
-        <v>502</v>
+      <c r="C208" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="D208" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="E208" s="10" t="s">
+        <v>493</v>
       </c>
       <c r="F208"/>
       <c r="G208" s="1">
@@ -68989,19 +68990,19 @@
     </row>
     <row r="209" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>155</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F209" s="1"/>
       <c r="G209" s="1">

</xml_diff>